<commit_message>
remove Low AFOLU file in spreadsheet- we are not using any add-on file for low AFOLU
</commit_message>
<xml_diff>
--- a/pic/RDM_strategy_uncertaity_xml_summary_20200510.xlsx
+++ b/pic/RDM_strategy_uncertaity_xml_summary_20200510.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NEXO-UA\Results\RDM_Colombia\scenario_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brinday\OneDrive - University of Maryland\UMD Research\2. Colombia RDM\Excel - data comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48569F6A-F418-46D4-A249-90A446CDB8F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{91D7BBC6-5292-434A-AFA2-EE0B6DA99210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{D0E2F046-9147-4F5F-8756-EEB02D665BE2}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D6B142E-5E8F-2446-85F5-F828CF9E4562}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <t>Strategy_1</t>
   </si>
@@ -99,6 +99,21 @@
     <t>Diet</t>
   </si>
   <si>
+    <t>Colombia_Public_Transport_High</t>
+  </si>
+  <si>
+    <t>transportation_UCD_CORE_ModEVsw</t>
+  </si>
+  <si>
+    <t>transportation_UCD_CORE_RapidEVsw_Colombia</t>
+  </si>
+  <si>
+    <t>land_constraint_Colombia_10_afforestation</t>
+  </si>
+  <si>
+    <t>Colombia_Low_Meat</t>
+  </si>
+  <si>
     <t>Strategy</t>
   </si>
   <si>
@@ -108,170 +123,175 @@
     <t>Origial High Ambition XML Name</t>
   </si>
   <si>
+    <t>Strategy_1_High_RPS
+Strategy_1_High_Nuclear</t>
+  </si>
+  <si>
     <t>Original Low Ambition XML Name</t>
   </si>
   <si>
+    <t>Strategy_1_Low_RPS
+Strategy_1_Low_Nuclear</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NEW </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>High</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ambition XML Name</t>
+    </r>
+  </si>
+  <si>
+    <t>Strategy_3_High_ElecTrans</t>
+  </si>
+  <si>
+    <t>Strategy_3_Low_ElecTrans</t>
+  </si>
+  <si>
+    <t>Strategy_4_High_PublicTrans</t>
+  </si>
+  <si>
+    <t>Strategy_5_High_AFOLU</t>
+  </si>
+  <si>
+    <t>Strategy_4_Low_PublicTrans</t>
+  </si>
+  <si>
+    <t>Colombia_GDP_High
+Colombia_Population_High</t>
+  </si>
+  <si>
+    <t>Colombia_GDP_Low
+Colombia_Population_Low</t>
+  </si>
+  <si>
+    <t>Global_CCS_Cost_High</t>
+  </si>
+  <si>
+    <t>Global_CCS_Cost_Normal</t>
+  </si>
+  <si>
+    <t>ag_prodchange_rcp2p6_hadgem2_pdssat
+hydro_impacts_HadGEM2-ES_rcp2p6
+runoff_impacts_HadGEM2-ES_rcp2p6</t>
+  </si>
+  <si>
+    <t>ag_prodchange_rcp2p6_gfdl_pdssat
+hydro_impacts_GFDL-ESM2M_rcp2p6
+runoff_impacts_GFDL-ESM2M_rcp2p6</t>
+  </si>
+  <si>
+    <t>Global_ag_trade_HOV_CL_25</t>
+  </si>
+  <si>
+    <t>Uncertainty_1_Low_GDP
+Uncertainty_1_Low_Population</t>
+  </si>
+  <si>
+    <t>Uncertainty_1_High_GDP
+Uncertainty_1_High_Population</t>
+  </si>
+  <si>
+    <t>Uncertainty_5_High_Ag
+Uncertainty_5_High_Hydro
+Uncertainty_5_High_Runnoff</t>
+  </si>
+  <si>
+    <t>Uncertainty_5_Low_Ag
+Uncertainty_5_Low_Hydro
+Uncertainty_5_Low_Runnoff</t>
+  </si>
+  <si>
     <t>Uncertainty</t>
   </si>
   <si>
     <t>NEW Low Ambition XML Name</t>
+  </si>
+  <si>
+    <t>Strategy_6_High_Meat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+transportation_UCD_CORE_RapidEVcost_Colombia_noPubTrninterp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+transportation_UCD_CORE_ModEVcost_Colombia_noPubTrninterp</t>
+  </si>
+  <si>
+    <t>Uncertainty_6_High_HOV-CL</t>
+  </si>
+  <si>
+    <t>Colombia_Public_Transport_Normal</t>
   </si>
   <si>
     <t>Solar_adv.xml
 Wind_adv.xml</t>
   </si>
   <si>
-    <t>NEW High Ambition XML Name</t>
-  </si>
-  <si>
-    <t>Colombia_RPS_High.xml
-Colombia_Nuclear_Zero.xml</t>
-  </si>
-  <si>
-    <t>Colombia_Bldg_ShellApplianceEff_High.xml
-Colombia_IndustrialEff_High.xml</t>
-  </si>
-  <si>
-    <t>transportation_UCD_CORE_RapidEVsw_Colombia.xml</t>
-  </si>
-  <si>
-    <t>Colombia_Public_Transport_High.xml</t>
-  </si>
-  <si>
-    <t>land_constraint_Colombia_10_afforestation.xml</t>
-  </si>
-  <si>
-    <t>Colombia_Low_Meat.xml</t>
-  </si>
-  <si>
-    <t>Strategy_1_High_RPS.xml
-Strategy_1_High_Nuclear.xml</t>
-  </si>
-  <si>
-    <t>Strategy_2_High_BldEE.xml
-Strategy_2_High_IndEE.xml</t>
-  </si>
-  <si>
-    <t>Strategy_3_High_ElecTrans.xml</t>
-  </si>
-  <si>
-    <t>Strategy_4_High_PublicTrans.xml</t>
-  </si>
-  <si>
-    <t>Strategy_5_High_AFOLU.xml</t>
-  </si>
-  <si>
-    <t>Strategy_6_High_Meat.xml</t>
-  </si>
-  <si>
-    <t>Colombia_RPS_Low.xml
-Colombia_Nuclear_Normal.xml</t>
-  </si>
-  <si>
-    <t>Colombia_Bldg_ShellApplianceEff_Low.xml
-Colombia_IndustrialEff_Low.xml</t>
-  </si>
-  <si>
-    <t>transportation_UCD_CORE_ModEVsw.xml</t>
-  </si>
-  <si>
-    <t>Colombia_Public_Transport_Normal.xml</t>
-  </si>
-  <si>
-    <t>land_constraint_Colombia_constant.xml</t>
-  </si>
-  <si>
-    <t>Strategy_1_Low_RPS.xml
-Strategy_1_Low_Nuclear.xml</t>
-  </si>
-  <si>
-    <t>Strategy_2_Low_BldEE.xml
-Strategy_2_Low_IndEE.xml</t>
-  </si>
-  <si>
-    <t>Strategy_3_Low_ElecTrans.xml</t>
-  </si>
-  <si>
-    <t>Strategy_4_Low_PublicTrans.xml</t>
-  </si>
-  <si>
-    <t>Strategy_5_Low_AFOLU.xml</t>
-  </si>
-  <si>
-    <t>Colombia_GDP_High.xml
-Colombia_Population_High.xml</t>
-  </si>
-  <si>
-    <t>transportation_UCD_CORE_RapidEVcost_Colombia_noPubTrninterp.xml</t>
-  </si>
-  <si>
-    <t>Global_CCS_Cost_Normal.xml</t>
-  </si>
-  <si>
-    <t>ag_prodchange_rcp2p6_gfdl_pdssat.xml
-hydro_impacts_GFDL-ESM2M_rcp2p6.xml
-runoff_impacts_GFDL-ESM2M_rcp2p6.xml</t>
-  </si>
-  <si>
-    <t>Global_ag_trade_HOV_CL_25.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_1_High_GDP.xml
-Uncertainty_1_High_Population.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_3_High_RECostSolar.xml Uncertainty_3_High_RECostWind.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_4_High_CCSCost.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_5_High_Ag.xml
-Uncertainty_5_High_Hydro.xml
-Uncertainty_5_High_Runnoff.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_6_High_HOV-CL.xml</t>
-  </si>
-  <si>
-    <t>Colombia_GDP_Low.xml
-Colombia_Population_Low.xml</t>
-  </si>
-  <si>
-    <t>transportation_UCD_CORE_ModEVcost_Colombia_noPubTrninterp.xml</t>
-  </si>
-  <si>
-    <t>Global_CCS_Cost_High.xml</t>
-  </si>
-  <si>
-    <t>ag_prodchange_rcp2p6_hadgem2_pdssat.xml
-hydro_impacts_HadGEM2-ES_rcp2p6.xml
-runoff_impacts_HadGEM2-ES_rcp2p6.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_1_Low_GDP.xml
-Uncertainty_1_Low_Population.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_2_Low_EVCost.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_4_Low_CCSCost.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_5_Low_Ag.xml
-Uncertainty_5_Low_Hydro.xml
-Uncertainty_5_Low_Runnoff.xml</t>
-  </si>
-  <si>
-    <t>Uncertainty_2_High_EVCost.xml</t>
+    <t>Colombia_Bldg_ShellApplianceEff_High
+Colombia_IndustrialEff_High</t>
+  </si>
+  <si>
+    <t>Colombia_Bldg_ShellApplianceEff_Low
+Colombia_IndustrialEff_Low</t>
+  </si>
+  <si>
+    <t>Uncertainty_4_High_CCSCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty_2_High_EVCost
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty_2_Low_EVCost
+</t>
+  </si>
+  <si>
+    <t>Uncertainty_4_Low_CCSCost</t>
+  </si>
+  <si>
+    <t>Strategy_2_High_BldEE
+Strategy_2_High_IndEE</t>
+  </si>
+  <si>
+    <t>Strategy_2_Low_BldEE
+Strategy_2_Low_IndEE</t>
+  </si>
+  <si>
+    <t>Colombia_RPS_Low
+Colombia_Nuclear_Normal</t>
+  </si>
+  <si>
+    <t>Colombia_RPS_High
+Colombia_Nuclear_Zero</t>
+  </si>
+  <si>
+    <t>Uncertainty_3_High_RECostSolar Uncertainty_3_High_RECostWind</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,6 +304,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri (Body)"/>
     </font>
     <font>
       <sz val="12"/>
@@ -372,19 +398,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -722,43 +748,42 @@
   <dimension ref="B3:H20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
     <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.25" customWidth="1"/>
-    <col min="4" max="4" width="45.75" customWidth="1"/>
-    <col min="5" max="5" width="32.375" customWidth="1"/>
-    <col min="6" max="6" width="38.125" customWidth="1"/>
-    <col min="7" max="7" width="30.75" customWidth="1"/>
+    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.125" customWidth="1"/>
+    <col min="6" max="6" width="36.5" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8">
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="31.5">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -766,20 +791,20 @@
         <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="31.5">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -787,19 +812,19 @@
         <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -807,19 +832,19 @@
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -827,19 +852,19 @@
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -847,19 +872,15 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="2:8">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -867,35 +888,35 @@
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8">
       <c r="B12" s="5" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="31.5">
       <c r="B13" s="12" t="s">
         <v>6</v>
       </c>
@@ -903,19 +924,19 @@
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="47.25">
       <c r="B14" s="12" t="s">
         <v>7</v>
       </c>
@@ -926,16 +947,16 @@
         <v>55</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="63" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="31.5">
       <c r="B15" s="12" t="s">
         <v>8</v>
       </c>
@@ -943,16 +964,16 @@
         <v>13</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="8"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8">
       <c r="B16" s="12" t="s">
         <v>9</v>
       </c>
@@ -960,19 +981,19 @@
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="63" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="47.25">
       <c r="B17" s="12" t="s">
         <v>10</v>
       </c>
@@ -980,19 +1001,19 @@
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
       <c r="B18" s="12" t="s">
         <v>16</v>
       </c>
@@ -1000,15 +1021,15 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="C20" s="9"/>
     </row>
   </sheetData>
@@ -1019,6 +1040,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A4312479EF03E04E9C80EFDBABE84330" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6a063b846935b1c24e04084d225ec4fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a7773017-533a-4fac-8654-0c9df14258d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ac990fe54ee2dfc432706ff1408291d" ns3:_="">
     <xsd:import namespace="a7773017-533a-4fac-8654-0c9df14258d0"/>
@@ -1196,7 +1223,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1205,13 +1232,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC5E852-43CE-4395-AE2E-08BA3FC088F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C53095-6DBC-4A4F-8FE7-1E052F02F02E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1229,26 +1266,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08564DE-8754-496E-B25E-7C4C54B72013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC5E852-43CE-4395-AE2E-08BA3FC088F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update script to remove Low AFOLU file in the output configuration
</commit_message>
<xml_diff>
--- a/pic/RDM_strategy_uncertaity_xml_summary_20200510.xlsx
+++ b/pic/RDM_strategy_uncertaity_xml_summary_20200510.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brinday\OneDrive - University of Maryland\UMD Research\2. Colombia RDM\Excel - data comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NEXO-UA\Github\IDB_RDM_Colombia\pic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{91D7BBC6-5292-434A-AFA2-EE0B6DA99210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{D0E2F046-9147-4F5F-8756-EEB02D665BE2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501663BA-4304-4D27-AB46-ABE4511F8F30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D6B142E-5E8F-2446-85F5-F828CF9E4562}"/>
   </bookViews>
@@ -99,21 +99,6 @@
     <t>Diet</t>
   </si>
   <si>
-    <t>Colombia_Public_Transport_High</t>
-  </si>
-  <si>
-    <t>transportation_UCD_CORE_ModEVsw</t>
-  </si>
-  <si>
-    <t>transportation_UCD_CORE_RapidEVsw_Colombia</t>
-  </si>
-  <si>
-    <t>land_constraint_Colombia_10_afforestation</t>
-  </si>
-  <si>
-    <t>Colombia_Low_Meat</t>
-  </si>
-  <si>
     <t>Strategy</t>
   </si>
   <si>
@@ -123,15 +108,7 @@
     <t>Origial High Ambition XML Name</t>
   </si>
   <si>
-    <t>Strategy_1_High_RPS
-Strategy_1_High_Nuclear</t>
-  </si>
-  <si>
     <t>Original Low Ambition XML Name</t>
-  </si>
-  <si>
-    <t>Strategy_1_Low_RPS
-Strategy_1_Low_Nuclear</t>
   </si>
   <si>
     <r>
@@ -159,132 +136,151 @@
     </r>
   </si>
   <si>
-    <t>Strategy_3_High_ElecTrans</t>
-  </si>
-  <si>
-    <t>Strategy_3_Low_ElecTrans</t>
-  </si>
-  <si>
-    <t>Strategy_4_High_PublicTrans</t>
-  </si>
-  <si>
-    <t>Strategy_5_High_AFOLU</t>
-  </si>
-  <si>
-    <t>Strategy_4_Low_PublicTrans</t>
-  </si>
-  <si>
-    <t>Colombia_GDP_High
-Colombia_Population_High</t>
-  </si>
-  <si>
-    <t>Colombia_GDP_Low
-Colombia_Population_Low</t>
-  </si>
-  <si>
-    <t>Global_CCS_Cost_High</t>
-  </si>
-  <si>
-    <t>Global_CCS_Cost_Normal</t>
-  </si>
-  <si>
-    <t>ag_prodchange_rcp2p6_hadgem2_pdssat
-hydro_impacts_HadGEM2-ES_rcp2p6
-runoff_impacts_HadGEM2-ES_rcp2p6</t>
-  </si>
-  <si>
-    <t>ag_prodchange_rcp2p6_gfdl_pdssat
-hydro_impacts_GFDL-ESM2M_rcp2p6
-runoff_impacts_GFDL-ESM2M_rcp2p6</t>
-  </si>
-  <si>
-    <t>Global_ag_trade_HOV_CL_25</t>
-  </si>
-  <si>
-    <t>Uncertainty_1_Low_GDP
-Uncertainty_1_Low_Population</t>
-  </si>
-  <si>
-    <t>Uncertainty_1_High_GDP
-Uncertainty_1_High_Population</t>
-  </si>
-  <si>
-    <t>Uncertainty_5_High_Ag
-Uncertainty_5_High_Hydro
-Uncertainty_5_High_Runnoff</t>
-  </si>
-  <si>
-    <t>Uncertainty_5_Low_Ag
-Uncertainty_5_Low_Hydro
-Uncertainty_5_Low_Runnoff</t>
-  </si>
-  <si>
     <t>Uncertainty</t>
   </si>
   <si>
     <t>NEW Low Ambition XML Name</t>
   </si>
   <si>
-    <t>Strategy_6_High_Meat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-transportation_UCD_CORE_RapidEVcost_Colombia_noPubTrninterp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-transportation_UCD_CORE_ModEVcost_Colombia_noPubTrninterp</t>
-  </si>
-  <si>
-    <t>Uncertainty_6_High_HOV-CL</t>
-  </si>
-  <si>
-    <t>Colombia_Public_Transport_Normal</t>
+    <t>Colombia_RPS_High.xml
+Colombia_Nuclear_Zero.xml</t>
+  </si>
+  <si>
+    <t>Colombia_Bldg_ShellApplianceEff_High.xml
+Colombia_IndustrialEff_High.xml</t>
+  </si>
+  <si>
+    <t>transportation_UCD_CORE_RapidEVsw_Colombia.xml</t>
+  </si>
+  <si>
+    <t>Colombia_Public_Transport_High.xml</t>
+  </si>
+  <si>
+    <t>land_constraint_Colombia_10_afforestation.xml</t>
+  </si>
+  <si>
+    <t>Colombia_Low_Meat.xml</t>
+  </si>
+  <si>
+    <t>Colombia_GDP_High.xml
+Colombia_Population_High.xml</t>
+  </si>
+  <si>
+    <t>transportation_UCD_CORE_RapidEVcost_Colombia_noPubTrninterp.xml</t>
   </si>
   <si>
     <t>Solar_adv.xml
 Wind_adv.xml</t>
   </si>
   <si>
-    <t>Colombia_Bldg_ShellApplianceEff_High
-Colombia_IndustrialEff_High</t>
-  </si>
-  <si>
-    <t>Colombia_Bldg_ShellApplianceEff_Low
-Colombia_IndustrialEff_Low</t>
-  </si>
-  <si>
-    <t>Uncertainty_4_High_CCSCost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty_2_High_EVCost
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty_2_Low_EVCost
-</t>
-  </si>
-  <si>
-    <t>Uncertainty_4_Low_CCSCost</t>
-  </si>
-  <si>
-    <t>Strategy_2_High_BldEE
-Strategy_2_High_IndEE</t>
-  </si>
-  <si>
-    <t>Strategy_2_Low_BldEE
-Strategy_2_Low_IndEE</t>
-  </si>
-  <si>
-    <t>Colombia_RPS_Low
-Colombia_Nuclear_Normal</t>
-  </si>
-  <si>
-    <t>Colombia_RPS_High
-Colombia_Nuclear_Zero</t>
-  </si>
-  <si>
-    <t>Uncertainty_3_High_RECostSolar Uncertainty_3_High_RECostWind</t>
+    <t>Global_CCS_Cost_Normal.xml</t>
+  </si>
+  <si>
+    <t>ag_prodchange_rcp2p6_gfdl_pdssat.xml
+hydro_impacts_GFDL-ESM2M_rcp2p6.xml
+runoff_impacts_GFDL-ESM2M_rcp2p6.xml</t>
+  </si>
+  <si>
+    <t>Global_ag_trade_HOV_CL_25.xml</t>
+  </si>
+  <si>
+    <t>Strategy_1_High_RPS.xml
+Strategy_1_High_Nuclear.xml</t>
+  </si>
+  <si>
+    <t>Strategy_2_High_BldEE.xml
+Strategy_2_High_IndEE.xml</t>
+  </si>
+  <si>
+    <t>Strategy_3_High_ElecTrans.xml</t>
+  </si>
+  <si>
+    <t>Strategy_4_High_PublicTrans.xml</t>
+  </si>
+  <si>
+    <t>Strategy_5_High_AFOLU.xml</t>
+  </si>
+  <si>
+    <t>Strategy_6_High_Meat.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_1_High_GDP.xml
+Uncertainty_1_High_Population.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_2_High_EVCost.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_3_High_RECostSolar.xml Uncertainty_3_High_RECostWind.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_4_High_CCSCost.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_5_High_Ag.xml
+Uncertainty_5_High_Hydro.xml
+Uncertainty_5_High_Runoff.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_6_High_HOV-CL.xml</t>
+  </si>
+  <si>
+    <t>Colombia_RPS_Low.xml
+Colombia_Nuclear_Normal.xml</t>
+  </si>
+  <si>
+    <t>Colombia_Bldg_ShellApplianceEff_Low.xml
+Colombia_IndustrialEff_Low.xml</t>
+  </si>
+  <si>
+    <t>transportation_UCD_CORE_ModEVsw.xml</t>
+  </si>
+  <si>
+    <t>Colombia_Public_Transport_Normal.xml</t>
+  </si>
+  <si>
+    <t>Colombia_GDP_Low.xml
+Colombia_Population_Low.xml</t>
+  </si>
+  <si>
+    <t>transportation_UCD_CORE_ModEVcost_Colombia_noPubTrninterp.xml</t>
+  </si>
+  <si>
+    <t>Global_CCS_Cost_High.xml</t>
+  </si>
+  <si>
+    <t>ag_prodchange_rcp2p6_hadgem2_pdssat.xml
+hydro_impacts_HadGEM2-ES_rcp2p6.xml
+runoff_impacts_HadGEM2-ES_rcp2p6.xml</t>
+  </si>
+  <si>
+    <t>Strategy_1_Low_RPS.xml
+Strategy_1_Low_Nuclear.xml</t>
+  </si>
+  <si>
+    <t>Strategy_2_Low_BldEE.xml
+Strategy_2_Low_IndEE.xml</t>
+  </si>
+  <si>
+    <t>Strategy_3_Low_ElecTrans.xml</t>
+  </si>
+  <si>
+    <t>Strategy_4_Low_PublicTrans.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_1_Low_GDP.xml
+Uncertainty_1_Low_Population.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_2_Low_EVCost.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_4_Low_CCSCost.xml</t>
+  </si>
+  <si>
+    <t>Uncertainty_5_Low_Ag.xml
+Uncertainty_5_Low_Hydro.xml
+Uncertainty_5_Low_Runoff.xml</t>
   </si>
 </sst>
 </file>
@@ -748,39 +744,39 @@
   <dimension ref="B3:H20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.125" customWidth="1"/>
-    <col min="6" max="6" width="36.5" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.125" customWidth="1"/>
+    <col min="5" max="5" width="32.5" customWidth="1"/>
+    <col min="6" max="6" width="39.125" customWidth="1"/>
+    <col min="7" max="7" width="30.25" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
       <c r="B3" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="31.5">
@@ -791,16 +787,16 @@
         <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="H4" s="10"/>
     </row>
@@ -812,16 +808,16 @@
         <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:8">
@@ -832,16 +828,16 @@
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:8">
@@ -852,16 +848,16 @@
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:8">
@@ -872,10 +868,10 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="8"/>
@@ -888,32 +884,32 @@
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="8"/>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="5" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="31.5">
@@ -924,19 +920,19 @@
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="47.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="31.5">
       <c r="B14" s="12" t="s">
         <v>7</v>
       </c>
@@ -944,16 +940,16 @@
         <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="31.5">
@@ -964,10 +960,10 @@
         <v>13</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="8"/>
@@ -981,16 +977,16 @@
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="47.25">
@@ -1001,16 +997,16 @@
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:7">
@@ -1021,10 +1017,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="8"/>

</xml_diff>